<commit_message>
lapdat + kim long
</commit_message>
<xml_diff>
--- a/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2023/Thang4/2.XuLyBH/XLBH2304_KimLong.xlsx
+++ b/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2023/Thang4/2.XuLyBH/XLBH2304_KimLong.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="74">
   <si>
     <t>STT</t>
   </si>
@@ -232,6 +232,27 @@
   </si>
   <si>
     <t>H</t>
+  </si>
+  <si>
+    <t>Thiết bị không check được nhiệt độ</t>
+  </si>
+  <si>
+    <t>Đổi thiết bị mới</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>Tùng</t>
+  </si>
+  <si>
+    <t>Thay IC giao tiếp, xử lý lại main + dây kết nối</t>
+  </si>
+  <si>
+    <t>BT</t>
+  </si>
+  <si>
+    <t>ID mới: 150220230042</t>
   </si>
 </sst>
 </file>
@@ -637,6 +658,30 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -654,30 +699,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -989,7 +1010,7 @@
   <dimension ref="A1:X114"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1021,41 +1042,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69"/>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
-      <c r="S1" s="69"/>
-      <c r="T1" s="69"/>
-      <c r="U1" s="69"/>
-      <c r="V1" s="69"/>
+      <c r="A1" s="77"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
       <c r="W1" s="36"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="72" t="s">
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="72"/>
+      <c r="F2" s="80"/>
       <c r="G2" s="4"/>
       <c r="H2" s="17"/>
       <c r="I2" s="40"/>
@@ -1088,57 +1109,57 @@
       <c r="V3" s="21"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="68" t="s">
+      <c r="A4" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68" t="s">
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="68"/>
-      <c r="L4" s="74" t="s">
+      <c r="K4" s="76"/>
+      <c r="L4" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="74" t="s">
+      <c r="M4" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="74" t="s">
+      <c r="N4" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="74" t="s">
+      <c r="O4" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="79" t="s">
+      <c r="P4" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="74" t="s">
+      <c r="Q4" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="74" t="s">
+      <c r="R4" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="81" t="s">
+      <c r="S4" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="U4" s="68" t="s">
+      <c r="U4" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="68" t="s">
+      <c r="V4" s="76" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="37"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="73"/>
+      <c r="A5" s="81"/>
       <c r="B5" s="67" t="s">
         <v>1</v>
       </c>
@@ -1169,16 +1190,16 @@
       <c r="K5" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="75"/>
-      <c r="M5" s="75"/>
-      <c r="N5" s="75"/>
-      <c r="O5" s="75"/>
-      <c r="P5" s="80"/>
-      <c r="Q5" s="75"/>
-      <c r="R5" s="75"/>
-      <c r="S5" s="81"/>
-      <c r="U5" s="68"/>
-      <c r="V5" s="68"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="74"/>
+      <c r="P5" s="72"/>
+      <c r="Q5" s="74"/>
+      <c r="R5" s="74"/>
+      <c r="S5" s="75"/>
+      <c r="U5" s="76"/>
+      <c r="V5" s="76"/>
       <c r="W5" s="37"/>
     </row>
     <row r="6" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1188,7 +1209,9 @@
       <c r="B6" s="58">
         <v>45027</v>
       </c>
-      <c r="C6" s="58"/>
+      <c r="C6" s="58">
+        <v>45028</v>
+      </c>
       <c r="D6" s="46" t="s">
         <v>57</v>
       </c>
@@ -1199,20 +1222,30 @@
       <c r="G6" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="H6" s="46"/>
+      <c r="H6" s="46" t="s">
+        <v>73</v>
+      </c>
       <c r="I6" s="59"/>
       <c r="J6" s="59"/>
       <c r="K6" s="62"/>
-      <c r="L6" s="62"/>
-      <c r="M6" s="62"/>
+      <c r="L6" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="M6" s="62" t="s">
+        <v>68</v>
+      </c>
       <c r="N6" s="60"/>
-      <c r="O6" s="60"/>
-      <c r="P6" s="62"/>
+      <c r="O6" s="60" t="s">
+        <v>69</v>
+      </c>
+      <c r="P6" s="62" t="s">
+        <v>70</v>
+      </c>
       <c r="Q6" s="60"/>
       <c r="R6" s="63"/>
       <c r="S6" s="64"/>
       <c r="T6" s="66"/>
-      <c r="U6" s="76" t="s">
+      <c r="U6" s="68" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -1227,7 +1260,9 @@
       <c r="B7" s="58">
         <v>45027</v>
       </c>
-      <c r="C7" s="58"/>
+      <c r="C7" s="58">
+        <v>45028</v>
+      </c>
       <c r="D7" s="46" t="s">
         <v>57</v>
       </c>
@@ -1242,16 +1277,28 @@
       <c r="I7" s="59"/>
       <c r="J7" s="61"/>
       <c r="K7" s="61"/>
-      <c r="L7" s="61"/>
-      <c r="M7" s="62"/>
+      <c r="L7" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="M7" s="62" t="s">
+        <v>71</v>
+      </c>
       <c r="N7" s="60"/>
-      <c r="O7" s="60"/>
-      <c r="P7" s="62"/>
-      <c r="Q7" s="60"/>
-      <c r="R7" s="63"/>
+      <c r="O7" s="60" t="s">
+        <v>72</v>
+      </c>
+      <c r="P7" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q7" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="R7" s="63" t="s">
+        <v>30</v>
+      </c>
       <c r="S7" s="64"/>
       <c r="T7" s="66"/>
-      <c r="U7" s="77"/>
+      <c r="U7" s="69"/>
       <c r="V7" s="3" t="s">
         <v>21</v>
       </c>
@@ -1264,7 +1311,9 @@
       <c r="B8" s="58">
         <v>45027</v>
       </c>
-      <c r="C8" s="58"/>
+      <c r="C8" s="58">
+        <v>45028</v>
+      </c>
       <c r="D8" s="46" t="s">
         <v>57</v>
       </c>
@@ -1279,16 +1328,28 @@
       <c r="I8" s="59"/>
       <c r="J8" s="60"/>
       <c r="K8" s="61"/>
-      <c r="L8" s="61"/>
-      <c r="M8" s="62"/>
+      <c r="L8" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="M8" s="62" t="s">
+        <v>71</v>
+      </c>
       <c r="N8" s="60"/>
-      <c r="O8" s="60"/>
-      <c r="P8" s="62"/>
-      <c r="Q8" s="60"/>
-      <c r="R8" s="63"/>
+      <c r="O8" s="60" t="s">
+        <v>72</v>
+      </c>
+      <c r="P8" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q8" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="R8" s="63" t="s">
+        <v>30</v>
+      </c>
       <c r="S8" s="64"/>
       <c r="T8" s="66"/>
-      <c r="U8" s="77"/>
+      <c r="U8" s="69"/>
       <c r="V8" s="3" t="s">
         <v>51</v>
       </c>
@@ -1301,7 +1362,9 @@
       <c r="B9" s="58">
         <v>45027</v>
       </c>
-      <c r="C9" s="58"/>
+      <c r="C9" s="58">
+        <v>45028</v>
+      </c>
       <c r="D9" s="46" t="s">
         <v>57</v>
       </c>
@@ -1316,16 +1379,28 @@
       <c r="I9" s="59"/>
       <c r="J9" s="65"/>
       <c r="K9" s="62"/>
-      <c r="L9" s="62"/>
-      <c r="M9" s="62"/>
+      <c r="L9" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="M9" s="62" t="s">
+        <v>71</v>
+      </c>
       <c r="N9" s="60"/>
-      <c r="O9" s="60"/>
-      <c r="P9" s="62"/>
-      <c r="Q9" s="60"/>
-      <c r="R9" s="63"/>
+      <c r="O9" s="60" t="s">
+        <v>72</v>
+      </c>
+      <c r="P9" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q9" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="R9" s="63" t="s">
+        <v>30</v>
+      </c>
       <c r="S9" s="64"/>
       <c r="T9" s="66"/>
-      <c r="U9" s="77"/>
+      <c r="U9" s="69"/>
       <c r="V9" s="3" t="s">
         <v>31</v>
       </c>
@@ -1354,7 +1429,7 @@
       <c r="R10" s="53"/>
       <c r="S10" s="55"/>
       <c r="T10" s="66"/>
-      <c r="U10" s="77"/>
+      <c r="U10" s="69"/>
       <c r="V10" s="3" t="s">
         <v>30</v>
       </c>
@@ -1383,7 +1458,7 @@
       <c r="R11" s="53"/>
       <c r="S11" s="3"/>
       <c r="T11" s="66"/>
-      <c r="U11" s="76" t="s">
+      <c r="U11" s="68" t="s">
         <v>19</v>
       </c>
       <c r="V11" s="3" t="s">
@@ -1414,7 +1489,7 @@
       <c r="R12" s="2"/>
       <c r="S12" s="3"/>
       <c r="T12" s="66"/>
-      <c r="U12" s="77"/>
+      <c r="U12" s="69"/>
       <c r="V12" s="3" t="s">
         <v>37</v>
       </c>
@@ -1443,7 +1518,7 @@
       <c r="R13" s="2"/>
       <c r="S13" s="3"/>
       <c r="T13" s="66"/>
-      <c r="U13" s="77"/>
+      <c r="U13" s="69"/>
       <c r="V13" s="3" t="s">
         <v>36</v>
       </c>
@@ -1472,7 +1547,7 @@
       <c r="R14" s="2"/>
       <c r="S14" s="3"/>
       <c r="T14" s="66"/>
-      <c r="U14" s="77"/>
+      <c r="U14" s="69"/>
       <c r="V14" s="3" t="s">
         <v>24</v>
       </c>
@@ -1501,7 +1576,7 @@
       <c r="R15" s="2"/>
       <c r="S15" s="3"/>
       <c r="T15" s="66"/>
-      <c r="U15" s="78"/>
+      <c r="U15" s="70"/>
       <c r="V15" s="3" t="s">
         <v>25</v>
       </c>
@@ -1651,7 +1726,7 @@
       </c>
       <c r="V20" s="3">
         <f>COUNTIF($Q$6:$Q$50,"PC")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W20" s="66"/>
     </row>
@@ -2223,7 +2298,7 @@
       </c>
       <c r="V39" s="3">
         <f>COUNTIF($O$6:$O$50,"*DM*")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W39" s="66"/>
     </row>
@@ -3202,13 +3277,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="U6:U10"/>
-    <mergeCell ref="U11:U15"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -3220,6 +3288,13 @@
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="L4:L5"/>
+    <mergeCell ref="U6:U10"/>
+    <mergeCell ref="U11:U15"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3263,41 +3338,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69"/>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
-      <c r="S1" s="69"/>
-      <c r="T1" s="69"/>
-      <c r="U1" s="69"/>
-      <c r="V1" s="69"/>
+      <c r="A1" s="77"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
       <c r="W1" s="36"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="72" t="s">
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="72"/>
+      <c r="F2" s="80"/>
       <c r="G2" s="4"/>
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
@@ -3330,57 +3405,57 @@
       <c r="V3" s="21"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="68" t="s">
+      <c r="A4" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68" t="s">
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="68" t="s">
+      <c r="K4" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="68"/>
-      <c r="M4" s="74" t="s">
+      <c r="L4" s="76"/>
+      <c r="M4" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="74" t="s">
+      <c r="N4" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="68" t="s">
+      <c r="O4" s="76" t="s">
         <v>7</v>
       </c>
       <c r="P4" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="68" t="s">
+      <c r="Q4" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="68" t="s">
+      <c r="R4" s="76" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="81" t="s">
+      <c r="S4" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="U4" s="68" t="s">
+      <c r="U4" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="68" t="s">
+      <c r="V4" s="76" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="37"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="73"/>
+      <c r="A5" s="81"/>
       <c r="B5" s="34" t="s">
         <v>1</v>
       </c>
@@ -3405,22 +3480,22 @@
       <c r="I5" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="68"/>
+      <c r="J5" s="76"/>
       <c r="K5" s="34" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="75"/>
-      <c r="N5" s="75"/>
-      <c r="O5" s="68"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="76"/>
       <c r="P5" s="82"/>
-      <c r="Q5" s="68"/>
-      <c r="R5" s="68"/>
-      <c r="S5" s="81"/>
-      <c r="U5" s="68"/>
-      <c r="V5" s="68"/>
+      <c r="Q5" s="76"/>
+      <c r="R5" s="76"/>
+      <c r="S5" s="75"/>
+      <c r="U5" s="76"/>
+      <c r="V5" s="76"/>
       <c r="W5" s="37"/>
     </row>
     <row r="6" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3446,7 +3521,7 @@
       <c r="R6" s="31"/>
       <c r="S6" s="3"/>
       <c r="T6" s="12"/>
-      <c r="U6" s="76" t="s">
+      <c r="U6" s="68" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -3477,7 +3552,7 @@
       <c r="R7" s="31"/>
       <c r="S7" s="3"/>
       <c r="T7" s="12"/>
-      <c r="U7" s="77"/>
+      <c r="U7" s="69"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -3506,7 +3581,7 @@
       <c r="R8" s="31"/>
       <c r="S8" s="3"/>
       <c r="T8" s="12"/>
-      <c r="U8" s="77"/>
+      <c r="U8" s="69"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -3535,7 +3610,7 @@
       <c r="R9" s="31"/>
       <c r="S9" s="3"/>
       <c r="T9" s="12"/>
-      <c r="U9" s="77"/>
+      <c r="U9" s="69"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -3564,7 +3639,7 @@
       <c r="R10" s="31"/>
       <c r="S10" s="3"/>
       <c r="T10" s="12"/>
-      <c r="U10" s="77"/>
+      <c r="U10" s="69"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -3593,7 +3668,7 @@
       <c r="R11" s="31"/>
       <c r="S11" s="3"/>
       <c r="T11" s="12"/>
-      <c r="U11" s="77"/>
+      <c r="U11" s="69"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -3622,7 +3697,7 @@
       <c r="R12" s="31"/>
       <c r="S12" s="3"/>
       <c r="T12" s="12"/>
-      <c r="U12" s="76" t="s">
+      <c r="U12" s="68" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -3653,7 +3728,7 @@
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
       <c r="T13" s="12"/>
-      <c r="U13" s="77"/>
+      <c r="U13" s="69"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -3682,7 +3757,7 @@
       <c r="R14" s="31"/>
       <c r="S14" s="3"/>
       <c r="T14" s="12"/>
-      <c r="U14" s="77"/>
+      <c r="U14" s="69"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -3711,7 +3786,7 @@
       <c r="R15" s="31"/>
       <c r="S15" s="3"/>
       <c r="T15" s="12"/>
-      <c r="U15" s="77"/>
+      <c r="U15" s="69"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -3740,7 +3815,7 @@
       <c r="R16" s="31"/>
       <c r="S16" s="3"/>
       <c r="T16" s="12"/>
-      <c r="U16" s="78"/>
+      <c r="U16" s="70"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -4971,13 +5046,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -4989,6 +5057,13 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>